<commit_message>
Mensaje descriptivo del cambio
</commit_message>
<xml_diff>
--- a/Base/Backlog_10.xlsx
+++ b/Base/Backlog_10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franciscoj\Python_Initial\Pyhton_Web\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73A76CC-A027-411D-99E9-8DB3D7289C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4817B2AD-7664-4FD2-9879-C91D78BC25E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
   </bookViews>
   <sheets>
     <sheet name="SPN" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
   <si>
     <t>Backlog</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Higor Cruz</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
   </si>
 </sst>
 </file>
@@ -159,12 +162,18 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -179,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,6 +237,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +568,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -599,73 +622,73 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="19">
         <v>2025</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="19">
         <v>10</v>
       </c>
-      <c r="E2" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F2" s="16">
+      <c r="E2" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F2" s="20">
         <v>45730</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="18">
         <v>326665</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="21">
         <v>45717</v>
       </c>
-      <c r="I2" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D3" s="19">
+        <v>10</v>
+      </c>
+      <c r="E3" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F3" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G3" s="18">
+        <v>327188</v>
+      </c>
+      <c r="H3" s="21">
+        <v>45719</v>
+      </c>
+      <c r="I3" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D3" s="8">
-        <v>10</v>
-      </c>
-      <c r="E3" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F3" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G3" s="12">
-        <v>327188</v>
-      </c>
-      <c r="H3" s="3">
-        <v>45719</v>
-      </c>
-      <c r="I3" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -821,7 +844,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -876,633 +899,633 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="19">
         <v>2025</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="19">
         <v>10</v>
       </c>
-      <c r="E2" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F2" s="16">
+      <c r="E2" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F2" s="20">
         <v>45730</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="18">
         <v>323755</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="21">
         <v>45689</v>
       </c>
-      <c r="I2" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="19">
         <v>2025</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="19">
         <v>10</v>
       </c>
-      <c r="E3" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F3" s="16">
+      <c r="E3" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F3" s="20">
         <v>45730</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="18">
         <v>326421</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="21">
         <v>45717</v>
       </c>
-      <c r="I3" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D4" s="19">
+        <v>10</v>
+      </c>
+      <c r="E4" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F4" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G4" s="18">
+        <v>326610</v>
+      </c>
+      <c r="H4" s="21">
+        <v>45717</v>
+      </c>
+      <c r="I4" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D5" s="19">
+        <v>10</v>
+      </c>
+      <c r="E5" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F5" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G5" s="18">
+        <v>326729</v>
+      </c>
+      <c r="H5" s="21">
+        <v>45717</v>
+      </c>
+      <c r="I5" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D6" s="19">
+        <v>10</v>
+      </c>
+      <c r="E6" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F6" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G6" s="18">
+        <v>327344</v>
+      </c>
+      <c r="H6" s="21">
+        <v>45717</v>
+      </c>
+      <c r="I6" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D7" s="19">
+        <v>10</v>
+      </c>
+      <c r="E7" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F7" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G7" s="18">
+        <v>324156</v>
+      </c>
+      <c r="H7" s="21">
+        <v>45689</v>
+      </c>
+      <c r="I7" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K7" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="8" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="B8" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="19">
         <v>2025</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D8" s="19">
         <v>10</v>
       </c>
-      <c r="E4" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F4" s="16">
+      <c r="E8" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F8" s="20">
         <v>45730</v>
       </c>
-      <c r="G4" s="12">
-        <v>326610</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G8" s="18">
+        <v>327101</v>
+      </c>
+      <c r="H8" s="21">
         <v>45717</v>
       </c>
-      <c r="I4" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="I8" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D9" s="19">
+        <v>10</v>
+      </c>
+      <c r="E9" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F9" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G9" s="18">
+        <v>327168</v>
+      </c>
+      <c r="H9" s="21">
+        <v>45717</v>
+      </c>
+      <c r="I9" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K9" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="10" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="19">
         <v>2025</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D10" s="19">
         <v>10</v>
       </c>
-      <c r="E5" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F5" s="16">
+      <c r="E10" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F10" s="20">
         <v>45730</v>
       </c>
-      <c r="G5" s="12">
-        <v>326729</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G10" s="18">
+        <v>325743</v>
+      </c>
+      <c r="H10" s="21">
+        <v>45689</v>
+      </c>
+      <c r="I10" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D11" s="19">
+        <v>10</v>
+      </c>
+      <c r="E11" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F11" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G11" s="18">
+        <v>327056</v>
+      </c>
+      <c r="H11" s="21">
         <v>45717</v>
       </c>
-      <c r="I5" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="I11" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D12" s="19">
+        <v>10</v>
+      </c>
+      <c r="E12" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F12" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G12" s="18">
+        <v>326324</v>
+      </c>
+      <c r="H12" s="21">
+        <v>45689</v>
+      </c>
+      <c r="I12" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J12" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K12" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="13" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B13" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="19">
         <v>2025</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D13" s="19">
         <v>10</v>
       </c>
-      <c r="E6" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F6" s="16">
+      <c r="E13" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F13" s="20">
         <v>45730</v>
       </c>
-      <c r="G6" s="12">
-        <v>327344</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G13" s="18">
+        <v>325625</v>
+      </c>
+      <c r="H13" s="21">
+        <v>45689</v>
+      </c>
+      <c r="I13" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D14" s="19">
+        <v>10</v>
+      </c>
+      <c r="E14" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F14" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G14" s="18">
+        <v>327214</v>
+      </c>
+      <c r="H14" s="21">
         <v>45717</v>
       </c>
-      <c r="I6" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="I14" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D15" s="19">
+        <v>10</v>
+      </c>
+      <c r="E15" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F15" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G15" s="18">
+        <v>327239</v>
+      </c>
+      <c r="H15" s="21">
+        <v>45717</v>
+      </c>
+      <c r="I15" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K15" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="16" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="19">
         <v>2025</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D16" s="19">
         <v>10</v>
       </c>
-      <c r="E7" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F7" s="16">
+      <c r="E16" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F16" s="20">
         <v>45730</v>
       </c>
-      <c r="G7" s="12">
-        <v>324156</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G16" s="18">
+        <v>325722</v>
+      </c>
+      <c r="H16" s="21">
+        <v>45717</v>
+      </c>
+      <c r="I16" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D17" s="19">
+        <v>10</v>
+      </c>
+      <c r="E17" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F17" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G17" s="18">
+        <v>325533</v>
+      </c>
+      <c r="H17" s="21">
         <v>45689</v>
       </c>
-      <c r="I7" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J7" s="8" t="s">
+      <c r="I17" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D18" s="19">
+        <v>10</v>
+      </c>
+      <c r="E18" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F18" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G18" s="18">
+        <v>327031</v>
+      </c>
+      <c r="H18" s="21">
+        <v>45717</v>
+      </c>
+      <c r="I18" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="19">
+        <v>2025</v>
+      </c>
+      <c r="D19" s="19">
+        <v>10</v>
+      </c>
+      <c r="E19" s="20">
+        <v>45726</v>
+      </c>
+      <c r="F19" s="20">
+        <v>45730</v>
+      </c>
+      <c r="G19" s="18">
+        <v>315817</v>
+      </c>
+      <c r="H19" s="21">
+        <v>45689</v>
+      </c>
+      <c r="I19" s="20">
+        <v>45726</v>
+      </c>
+      <c r="J19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D8" s="8">
-        <v>10</v>
-      </c>
-      <c r="E8" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F8" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G8" s="12">
-        <v>327101</v>
-      </c>
-      <c r="H8" s="3">
-        <v>45717</v>
-      </c>
-      <c r="I8" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D9" s="8">
-        <v>10</v>
-      </c>
-      <c r="E9" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F9" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G9" s="12">
-        <v>327168</v>
-      </c>
-      <c r="H9" s="3">
-        <v>45717</v>
-      </c>
-      <c r="I9" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D10" s="8">
-        <v>10</v>
-      </c>
-      <c r="E10" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F10" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G10" s="12">
-        <v>325743</v>
-      </c>
-      <c r="H10" s="3">
-        <v>45689</v>
-      </c>
-      <c r="I10" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D11" s="8">
-        <v>10</v>
-      </c>
-      <c r="E11" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F11" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G11" s="12">
-        <v>327056</v>
-      </c>
-      <c r="H11" s="3">
-        <v>45717</v>
-      </c>
-      <c r="I11" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D12" s="8">
-        <v>10</v>
-      </c>
-      <c r="E12" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F12" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G12" s="12">
-        <v>326324</v>
-      </c>
-      <c r="H12" s="3">
-        <v>45689</v>
-      </c>
-      <c r="I12" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D13" s="8">
-        <v>10</v>
-      </c>
-      <c r="E13" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F13" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G13" s="12">
-        <v>325625</v>
-      </c>
-      <c r="H13" s="3">
-        <v>45689</v>
-      </c>
-      <c r="I13" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D14" s="8">
-        <v>10</v>
-      </c>
-      <c r="E14" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F14" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G14" s="12">
-        <v>327214</v>
-      </c>
-      <c r="H14" s="3">
-        <v>45717</v>
-      </c>
-      <c r="I14" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D15" s="8">
-        <v>10</v>
-      </c>
-      <c r="E15" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F15" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G15" s="12">
-        <v>327239</v>
-      </c>
-      <c r="H15" s="3">
-        <v>45717</v>
-      </c>
-      <c r="I15" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D16" s="8">
-        <v>10</v>
-      </c>
-      <c r="E16" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F16" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G16" s="12">
-        <v>325722</v>
-      </c>
-      <c r="H16" s="3">
-        <v>45717</v>
-      </c>
-      <c r="I16" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D17" s="8">
-        <v>10</v>
-      </c>
-      <c r="E17" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F17" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G17" s="12">
-        <v>325533</v>
-      </c>
-      <c r="H17" s="3">
-        <v>45689</v>
-      </c>
-      <c r="I17" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D18" s="8">
-        <v>10</v>
-      </c>
-      <c r="E18" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F18" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G18" s="12">
-        <v>327031</v>
-      </c>
-      <c r="H18" s="3">
-        <v>45717</v>
-      </c>
-      <c r="I18" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D19" s="8">
-        <v>10</v>
-      </c>
-      <c r="E19" s="16">
-        <v>45726</v>
-      </c>
-      <c r="F19" s="16">
-        <v>45730</v>
-      </c>
-      <c r="G19" s="12">
-        <v>315817</v>
-      </c>
-      <c r="H19" s="3">
-        <v>45689</v>
-      </c>
-      <c r="I19" s="16">
-        <v>45726</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="18" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>